<commit_message>
Added command line for future
</commit_message>
<xml_diff>
--- a/src/main/java/net/jgp/books/spark/ch16/lab100_cache_checkpoint/Cache and checkpoint performance analysis (002).xlsx
+++ b/src/main/java/net/jgp/books/spark/ch16/lab100_cache_checkpoint/Cache and checkpoint performance analysis (002).xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgp/Workspaces/Book/net.jgp.books.spark.ch16/src/main/java/net/jgp/books/spark/ch16/lab100_cache_checkpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14301551-5C06-F749-ACF4-2F2F7B18304E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECEC037-F40D-FD4F-A11A-6D4BA8395742}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11140" yWindow="460" windowWidth="38580" windowHeight="42240" xr2:uid="{99E4B593-27CD-5046-B562-66C9A4DBDE3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chapter 16 - Lab 100 Benchmark" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -300,7 +300,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$48</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -335,7 +335,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$1:$S$1</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -380,7 +380,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$48:$S$48</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$48:$S$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -403,10 +403,10 @@
                   <c:v>18.581125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.725200000000001</c:v>
+                  <c:v>19.744583333333331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.888916666666667</c:v>
+                  <c:v>19.459208333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>16.013500000000001</c:v>
@@ -435,7 +435,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$49</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -470,7 +470,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$1:$S$1</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -515,7 +515,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$49:$S$49</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$49:$S$49</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -538,10 +538,10 @@
                   <c:v>12.238958333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.43455</c:v>
+                  <c:v>12.866766666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.700916666666666</c:v>
+                  <c:v>12.543208333333332</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10.587428571428573</c:v>
@@ -570,7 +570,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$50</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -605,7 +605,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$1:$S$1</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -650,7 +650,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$50:$S$50</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$50:$S$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -673,10 +673,10 @@
                   <c:v>10.124916666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.8902999999999999</c:v>
+                  <c:v>8.8194166666666671</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0338333333333338</c:v>
+                  <c:v>9.0915416666666662</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7.5805000000000007</c:v>
@@ -705,7 +705,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$51</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -740,7 +740,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$1:$S$1</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -785,7 +785,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$51:$S$51</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$H$51:$S$51</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
@@ -808,10 +808,10 @@
                   <c:v>10.068499999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>8.0960000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7.2845000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>7.5055714285714279</c:v>
@@ -1074,7 +1074,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$43</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1094,7 +1094,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$S$1</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$C$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1154,7 +1154,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$43:$S$43</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$C$43:$S$43</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1192,10 +1192,10 @@
                   <c:v>74324.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103626</c:v>
+                  <c:v>98722.916666666657</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>119333.5</c:v>
+                  <c:v>116755.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>112094.5</c:v>
@@ -1223,7 +1223,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$44</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1243,7 +1243,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$S$1</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$C$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1303,7 +1303,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$44:$S$44</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$C$44:$S$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1341,10 +1341,10 @@
                   <c:v>48955.833333333328</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>67172.75</c:v>
+                  <c:v>64333.833333333328</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76205.5</c:v>
+                  <c:v>75259.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>74112</c:v>
@@ -1372,7 +1372,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$45</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1392,7 +1392,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$S$1</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$C$1:$S$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1452,7 +1452,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$45:$S$45</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$C$45:$S$45</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1490,10 +1490,10 @@
                   <c:v>40499.666666666672</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44451.5</c:v>
+                  <c:v>44097.083333333328</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54203</c:v>
+                  <c:v>54549.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>53063.5</c:v>
@@ -1521,7 +1521,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$46</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$B$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1541,7 +1541,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$46:$S$46</c:f>
+              <c:f>'Chapter 16 - Lab 100 Benchmark'!$C$46:$S$46</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1579,10 +1579,10 @@
                   <c:v>40274</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>40480</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>43707</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>52539</c:v>
@@ -1732,47 +1732,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.58072375328083992"/>
-          <c:y val="0.66956583552055993"/>
-          <c:w val="0.32760634446556247"/>
-          <c:h val="4.6875328083989511E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3285,7 +3244,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
-      <selection pane="bottomRight" activeCell="O28" sqref="O28"/>
+      <selection pane="bottomRight" activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
@@ -3586,7 +3545,9 @@
       <c r="M8" s="6">
         <v>84295</v>
       </c>
-      <c r="N8" s="6"/>
+      <c r="N8" s="6">
+        <v>102992</v>
+      </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -3633,7 +3594,9 @@
       <c r="M9" s="6">
         <v>57848</v>
       </c>
-      <c r="N9" s="6"/>
+      <c r="N9" s="6">
+        <v>67581</v>
+      </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
@@ -3680,7 +3643,9 @@
       <c r="M10" s="6">
         <v>42495</v>
       </c>
-      <c r="N10" s="6"/>
+      <c r="N10" s="6">
+        <v>50049</v>
+      </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -3717,7 +3682,9 @@
         <v>25596</v>
       </c>
       <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="N11" s="6">
+        <v>47707</v>
+      </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -3967,7 +3934,7 @@
       </c>
       <c r="N18" s="2">
         <f t="shared" si="0"/>
-        <v>125011</v>
+        <v>114001.5</v>
       </c>
       <c r="O18" s="2">
         <f t="shared" si="0"/>
@@ -4038,7 +4005,7 @@
       </c>
       <c r="N19" s="2">
         <f t="shared" si="1"/>
-        <v>81679</v>
+        <v>74630</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="1"/>
@@ -4109,7 +4076,7 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" si="2"/>
-        <v>56736</v>
+        <v>53392.5</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" si="2"/>
@@ -4178,9 +4145,9 @@
         <f t="shared" si="3"/>
         <v>40274</v>
       </c>
-      <c r="N21" s="2" t="str">
+      <c r="N21" s="2">
         <f t="shared" si="3"/>
-        <v/>
+        <v>47707</v>
       </c>
       <c r="O21" s="2" t="str">
         <f t="shared" si="3"/>
@@ -4434,7 +4401,9 @@
       <c r="N28" s="6">
         <v>82448</v>
       </c>
-      <c r="O28" s="6"/>
+      <c r="O28" s="6">
+        <v>88944</v>
+      </c>
       <c r="P28" s="6">
         <v>115235</v>
       </c>
@@ -4469,7 +4438,9 @@
       <c r="N29" s="6">
         <v>52729</v>
       </c>
-      <c r="O29" s="6"/>
+      <c r="O29" s="6">
+        <v>61033</v>
+      </c>
       <c r="P29" s="6">
         <v>76861</v>
       </c>
@@ -4504,7 +4475,9 @@
       <c r="N30" s="6">
         <v>36718</v>
       </c>
-      <c r="O30" s="6"/>
+      <c r="O30" s="6">
+        <v>45547</v>
+      </c>
       <c r="P30" s="6">
         <v>52661</v>
       </c>
@@ -4535,7 +4508,9 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
+      <c r="O31" s="6">
+        <v>43707</v>
+      </c>
       <c r="P31" s="6">
         <v>52539</v>
       </c>
@@ -4586,7 +4561,9 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
+      <c r="N33" s="6">
+        <v>85851</v>
+      </c>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
@@ -4609,7 +4586,9 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
+      <c r="N34" s="6">
+        <v>56780</v>
+      </c>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="6"/>
@@ -4632,7 +4611,9 @@
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
+      <c r="N35" s="6">
+        <v>40071</v>
+      </c>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="6"/>
@@ -4655,7 +4636,9 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
+      <c r="N36" s="6">
+        <v>33253</v>
+      </c>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="6"/>
@@ -4736,11 +4719,11 @@
       </c>
       <c r="N38" s="2">
         <f t="shared" si="6"/>
-        <v>82241</v>
+        <v>83444.333333333328</v>
       </c>
       <c r="O38" s="2">
         <f t="shared" si="6"/>
-        <v>99257</v>
+        <v>94100.5</v>
       </c>
       <c r="P38" s="2">
         <f t="shared" ref="P38" si="7">IF(ISERROR(AVERAGE(P33,P28,P23)),"",AVERAGE(P33,P28,P23))</f>
@@ -4810,11 +4793,11 @@
       </c>
       <c r="N39" s="2">
         <f t="shared" si="11"/>
-        <v>52666.5</v>
+        <v>54037.666666666664</v>
       </c>
       <c r="O39" s="2">
         <f t="shared" si="11"/>
-        <v>64818</v>
+        <v>62925.5</v>
       </c>
       <c r="P39" s="2">
         <f t="shared" ref="P39" si="12">IF(ISERROR(AVERAGE(P34,P29,P24)),"",AVERAGE(P34,P29,P24))</f>
@@ -4884,11 +4867,11 @@
       </c>
       <c r="N40" s="2">
         <f t="shared" si="16"/>
-        <v>32167</v>
+        <v>34801.666666666664</v>
       </c>
       <c r="O40" s="2">
         <f t="shared" si="16"/>
-        <v>44162</v>
+        <v>44854.5</v>
       </c>
       <c r="P40" s="2">
         <f t="shared" ref="P40:P41" si="17">IF(ISERROR(AVERAGE(P35,P30,P25)),"",AVERAGE(P35,P30,P25))</f>
@@ -4956,13 +4939,13 @@
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="N41" s="2" t="str">
+      <c r="N41" s="2">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="O41" s="2" t="str">
+        <v>33253</v>
+      </c>
+      <c r="O41" s="2">
         <f t="shared" si="15"/>
-        <v/>
+        <v>43707</v>
       </c>
       <c r="P41" s="2">
         <f t="shared" si="17"/>
@@ -5034,11 +5017,11 @@
       </c>
       <c r="N43" s="2">
         <f t="shared" si="20"/>
-        <v>103626</v>
+        <v>98722.916666666657</v>
       </c>
       <c r="O43" s="2">
         <f t="shared" si="20"/>
-        <v>119333.5</v>
+        <v>116755.25</v>
       </c>
       <c r="P43" s="2">
         <f t="shared" si="20"/>
@@ -5108,11 +5091,11 @@
       </c>
       <c r="N44" s="2">
         <f t="shared" si="23"/>
-        <v>67172.75</v>
+        <v>64333.833333333328</v>
       </c>
       <c r="O44" s="2">
         <f t="shared" si="23"/>
-        <v>76205.5</v>
+        <v>75259.25</v>
       </c>
       <c r="P44" s="2">
         <f t="shared" si="23"/>
@@ -5182,11 +5165,11 @@
       </c>
       <c r="N45" s="2">
         <f t="shared" si="26"/>
-        <v>44451.5</v>
+        <v>44097.083333333328</v>
       </c>
       <c r="O45" s="2">
         <f t="shared" si="26"/>
-        <v>54203</v>
+        <v>54549.25</v>
       </c>
       <c r="P45" s="2">
         <f t="shared" si="26"/>
@@ -5254,13 +5237,13 @@
         <f t="shared" si="29"/>
         <v>40274</v>
       </c>
-      <c r="N46" s="2" t="e">
+      <c r="N46" s="2">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O46" s="2" t="e">
+        <v>40480</v>
+      </c>
+      <c r="O46" s="2">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>43707</v>
       </c>
       <c r="P46" s="2">
         <f t="shared" si="29"/>
@@ -5332,11 +5315,11 @@
       </c>
       <c r="N48" s="12">
         <f t="shared" si="30"/>
-        <v>20.725200000000001</v>
+        <v>19.744583333333331</v>
       </c>
       <c r="O48" s="12">
         <f t="shared" si="30"/>
-        <v>19.888916666666667</v>
+        <v>19.459208333333333</v>
       </c>
       <c r="P48" s="12">
         <f t="shared" si="30"/>
@@ -5406,11 +5389,11 @@
       </c>
       <c r="N49" s="12">
         <f t="shared" si="32"/>
-        <v>13.43455</v>
+        <v>12.866766666666667</v>
       </c>
       <c r="O49" s="12">
         <f t="shared" si="32"/>
-        <v>12.700916666666666</v>
+        <v>12.543208333333332</v>
       </c>
       <c r="P49" s="12">
         <f t="shared" si="32"/>
@@ -5480,11 +5463,11 @@
       </c>
       <c r="N50" s="12">
         <f t="shared" si="32"/>
-        <v>8.8902999999999999</v>
+        <v>8.8194166666666671</v>
       </c>
       <c r="O50" s="12">
         <f t="shared" si="32"/>
-        <v>9.0338333333333338</v>
+        <v>9.0915416666666662</v>
       </c>
       <c r="P50" s="12">
         <f t="shared" si="32"/>
@@ -5552,13 +5535,13 @@
         <f t="shared" si="32"/>
         <v>10.068499999999998</v>
       </c>
-      <c r="N51" s="12" t="e">
+      <c r="N51" s="12">
         <f t="shared" si="32"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O51" s="12" t="e">
+        <v>8.0960000000000001</v>
+      </c>
+      <c r="O51" s="12">
         <f t="shared" si="32"/>
-        <v>#DIV/0!</v>
+        <v>7.2845000000000004</v>
       </c>
       <c r="P51" s="12">
         <f t="shared" si="32"/>

</xml_diff>